<commit_message>
DNs. market data. 2030 and 2040. Upload.
</commit_message>
<xml_diff>
--- a/data/CS7/Market Data/CS7_market_data_2025.xlsx
+++ b/data/CS7/Market Data/CS7_market_data_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS7\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC176A8-D9AD-490C-AB44-5CC7F76133DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BD5C87-0BFA-416E-AD24-99B5E6807031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35790" yWindow="-11505" windowWidth="28800" windowHeight="15285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67080" yWindow="-12555" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -134,6 +134,9 @@
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Energy, Winter"/>
@@ -154,7 +157,7 @@
         </row>
         <row r="4">
           <cell r="B4">
-            <v>1.4999999999999999E-2</v>
+            <v>2.5000000000000001E-2</v>
           </cell>
         </row>
         <row r="5">
@@ -2225,8 +2228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2301,7 +2304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E73F7F-45E0-423B-A01B-B6DF6F75CAB7}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:Y4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Test. TN. 3 market scenarios.
</commit_message>
<xml_diff>
--- a/data/CS7/Market Data/CS7_market_data_2025.xlsx
+++ b/data/CS7/Market Data/CS7_market_data_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS7\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BD5C87-0BFA-416E-AD24-99B5E6807031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EFCED5-7477-49C2-938B-C843CB35713C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-12555" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-14400" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -2242,19 +2242,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>

<commit_message>
Test. 3 operation scenarios. MA57
</commit_message>
<xml_diff>
--- a/data/CS7/Market Data/CS7_market_data_2025.xlsx
+++ b/data/CS7/Market Data/CS7_market_data_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS7\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EFCED5-7477-49C2-938B-C843CB35713C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4887D6-6656-4A05-B77B-55E0DD19FB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-14400" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2242,19 +2242,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>

<commit_message>
Test. 9 operation scenarios. 3 market scenarios. MA97
</commit_message>
<xml_diff>
--- a/data/CS7/Market Data/CS7_market_data_2025.xlsx
+++ b/data/CS7/Market Data/CS7_market_data_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS7\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4887D6-6656-4A05-B77B-55E0DD19FB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F765DB-FCCF-41DB-96E6-1C95EEC3650E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-14400" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2242,19 +2242,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>

<commit_message>
Test. TN. 6 oper scenarios 2040, 2045
</commit_message>
<xml_diff>
--- a/data/CS7/Market Data/CS7_market_data_2025.xlsx
+++ b/data/CS7/Market Data/CS7_market_data_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS7\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842DB106-3645-4514-9731-76F964E6A89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089A678B-0662-4798-87F6-2EC6A3689B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-14400" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32595" yWindow="-9960" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -2229,7 +2229,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Test. TN and DNs. 3 oper scenarios
</commit_message>
<xml_diff>
--- a/data/CS7/Market Data/CS7_market_data_2025.xlsx
+++ b/data/CS7/Market Data/CS7_market_data_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS7\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089A678B-0662-4798-87F6-2EC6A3689B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CA9091-3C29-43D4-8EEF-68F632ED8D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32595" yWindow="-9960" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67080" yWindow="-12555" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -2229,7 +2229,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Detailed results OF added to results.
</commit_message>
<xml_diff>
--- a/data/CS7/Market Data/CS7_market_data_2025.xlsx
+++ b/data/CS7/Market Data/CS7_market_data_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS7\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1AD3D0-C8AC-4731-8947-BEE58C7E32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1988890D-E963-4059-B066-50710C62C430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-12555" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30195" yWindow="-12885" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Test. Different market scenario probability distribution.
</commit_message>
<xml_diff>
--- a/data/CS7/Market Data/CS7_market_data_2025.xlsx
+++ b/data/CS7/Market Data/CS7_market_data_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS7\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1988890D-E963-4059-B066-50710C62C430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D7714E-E213-4BDF-A879-F0C6F039DBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30195" yWindow="-12885" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30630" yWindow="-12450" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -2229,7 +2229,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2245,16 +2245,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="1">
-        <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>0.6</v>
       </c>
       <c r="D1" s="1">
-        <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>0.2</v>
       </c>
       <c r="E1" s="1">
-        <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>0.2</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>

<commit_message>
Regularization added to TN.
</commit_message>
<xml_diff>
--- a/data/CS7/Market Data/CS7_market_data_2025.xlsx
+++ b/data/CS7/Market Data/CS7_market_data_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS7\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67515543-A557-400C-88E5-5923640788BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF481DDF-9A2D-4C0E-8343-97B10D48D02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67080" yWindow="-12555" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -2229,7 +2229,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2245,13 +2245,16 @@
         <v>3</v>
       </c>
       <c r="C1" s="1">
-        <v>0.4</v>
+        <f>1/$B$1</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
-        <v>0.3</v>
+        <f t="shared" ref="D1:E1" si="0">1/$B$1</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E1" s="1">
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>

<commit_message>
Test. Planning new formulation
</commit_message>
<xml_diff>
--- a/data/CS7/Market Data/CS7_market_data_2025.xlsx
+++ b/data/CS7/Market Data/CS7_market_data_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS7\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49E2325-E60F-42F1-AA29-7AD579ED96E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9103BD7-FCCB-488A-BA24-7583F7D06D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72570" yWindow="3525" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="73005" yWindow="3960" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>

</xml_diff>